<commit_message>
Area de impresion ajustada_Seccion 11 finalizada
</commit_message>
<xml_diff>
--- a/31. 4BONUS - Imprimir Varias Páginas.xlsx.xlsx
+++ b/31. 4BONUS - Imprimir Varias Páginas.xlsx.xlsx
@@ -1,27 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Miguel Maraby\Video Cursos\Excel 2017\Producción\Excel y Word\BONOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PAUL\Downloads\Materiales-Para-Descargar\Curso_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2D20A2-57A5-47AD-B577-61315A777133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{ED4E87CF-F07F-4EB8-9F82-B30A4F153AAD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{ED4E87CF-F07F-4EB8-9F82-B30A4F153AAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla Ejercicio" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tabla Ejercicio'!$A$3:$F$42</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Tabla Ejercicio'!$3:$3</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -83,7 +94,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -181,16 +192,16 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -510,21 +521,21 @@
   <dimension ref="A3:F163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="12.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.3984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -544,7 +555,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -565,7 +576,7 @@
         <v>6693</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -586,7 +597,7 @@
         <v>8936</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -607,7 +618,7 @@
         <v>12472</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -628,7 +639,7 @@
         <v>3585</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -649,7 +660,7 @@
         <v>3585</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -670,7 +681,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
@@ -691,7 +702,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
@@ -712,7 +723,7 @@
         <v>4562</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
@@ -733,7 +744,7 @@
         <v>12472</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
@@ -754,7 +765,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
@@ -775,7 +786,7 @@
         <v>12965</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
@@ -796,7 +807,7 @@
         <v>10829</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>0</v>
       </c>
@@ -817,7 +828,7 @@
         <v>20629</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
@@ -838,7 +849,7 @@
         <v>4562</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
@@ -859,7 +870,7 @@
         <v>8972</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
@@ -880,7 +891,7 @@
         <v>8936</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>1</v>
       </c>
@@ -901,7 +912,7 @@
         <v>8936</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>0</v>
       </c>
@@ -922,7 +933,7 @@
         <v>4668</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>0</v>
       </c>
@@ -943,7 +954,7 @@
         <v>4631</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>3</v>
       </c>
@@ -964,7 +975,7 @@
         <v>3979</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>3</v>
       </c>
@@ -985,7 +996,7 @@
         <v>8701</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
@@ -1006,7 +1017,7 @@
         <v>11833</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>1</v>
       </c>
@@ -1027,7 +1038,7 @@
         <v>8701</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>2</v>
       </c>
@@ -1048,7 +1059,7 @@
         <v>4562</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
@@ -1069,7 +1080,7 @@
         <v>8972</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>2</v>
       </c>
@@ -1090,7 +1101,7 @@
         <v>3979</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>0</v>
       </c>
@@ -1111,7 +1122,7 @@
         <v>20629</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>0</v>
       </c>
@@ -1132,7 +1143,7 @@
         <v>8701</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>0</v>
       </c>
@@ -1153,7 +1164,7 @@
         <v>12965</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>3</v>
       </c>
@@ -1174,7 +1185,7 @@
         <v>12355</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>3</v>
       </c>
@@ -1195,7 +1206,7 @@
         <v>12355</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>3</v>
       </c>
@@ -1216,7 +1227,7 @@
         <v>20629</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>1</v>
       </c>
@@ -1237,7 +1248,7 @@
         <v>12472</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>1</v>
       </c>
@@ -1258,7 +1269,7 @@
         <v>11833</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>2</v>
       </c>
@@ -1279,7 +1290,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>2</v>
       </c>
@@ -1300,7 +1311,7 @@
         <v>11833</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>3</v>
       </c>
@@ -1321,7 +1332,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>1</v>
       </c>
@@ -1342,7 +1353,7 @@
         <v>4631</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A42" s="3" t="s">
         <v>1</v>
       </c>
@@ -1363,7 +1374,7 @@
         <v>12965</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>0</v>
       </c>
@@ -1384,7 +1395,7 @@
         <v>6693</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>0</v>
       </c>
@@ -1405,7 +1416,7 @@
         <v>8936</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="3" t="s">
         <v>0</v>
       </c>
@@ -1426,7 +1437,7 @@
         <v>12472</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
         <v>3</v>
       </c>
@@ -1447,7 +1458,7 @@
         <v>3585</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="3" t="s">
         <v>3</v>
       </c>
@@ -1468,7 +1479,7 @@
         <v>3585</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="3" t="s">
         <v>3</v>
       </c>
@@ -1489,7 +1500,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
         <v>3</v>
       </c>
@@ -1510,7 +1521,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
         <v>3</v>
       </c>
@@ -1531,7 +1542,7 @@
         <v>4562</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="3" t="s">
         <v>1</v>
       </c>
@@ -1552,7 +1563,7 @@
         <v>12472</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="3" t="s">
         <v>1</v>
       </c>
@@ -1573,7 +1584,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="3" t="s">
         <v>2</v>
       </c>
@@ -1594,7 +1605,7 @@
         <v>12965</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="3" t="s">
         <v>0</v>
       </c>
@@ -1615,7 +1626,7 @@
         <v>10829</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="3" t="s">
         <v>0</v>
       </c>
@@ -1636,7 +1647,7 @@
         <v>20629</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="3" t="s">
         <v>3</v>
       </c>
@@ -1657,7 +1668,7 @@
         <v>4562</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="3" t="s">
         <v>3</v>
       </c>
@@ -1678,7 +1689,7 @@
         <v>8972</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
         <v>3</v>
       </c>
@@ -1699,7 +1710,7 @@
         <v>8936</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="3" t="s">
         <v>1</v>
       </c>
@@ -1720,7 +1731,7 @@
         <v>8936</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="3" t="s">
         <v>0</v>
       </c>
@@ -1741,7 +1752,7 @@
         <v>4668</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="3" t="s">
         <v>0</v>
       </c>
@@ -1762,7 +1773,7 @@
         <v>4631</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="3" t="s">
         <v>3</v>
       </c>
@@ -1783,7 +1794,7 @@
         <v>3979</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="3" t="s">
         <v>3</v>
       </c>
@@ -1804,7 +1815,7 @@
         <v>8701</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="3" t="s">
         <v>3</v>
       </c>
@@ -1825,7 +1836,7 @@
         <v>11833</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
         <v>1</v>
       </c>
@@ -1846,7 +1857,7 @@
         <v>8701</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="3" t="s">
         <v>2</v>
       </c>
@@ -1867,7 +1878,7 @@
         <v>4562</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="3" t="s">
         <v>2</v>
       </c>
@@ -1888,7 +1899,7 @@
         <v>8972</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="3" t="s">
         <v>2</v>
       </c>
@@ -1909,7 +1920,7 @@
         <v>3979</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="3" t="s">
         <v>0</v>
       </c>
@@ -1930,7 +1941,7 @@
         <v>20629</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="3" t="s">
         <v>0</v>
       </c>
@@ -1951,7 +1962,7 @@
         <v>8701</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="3" t="s">
         <v>0</v>
       </c>
@@ -1972,7 +1983,7 @@
         <v>12965</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="3" t="s">
         <v>3</v>
       </c>
@@ -1993,7 +2004,7 @@
         <v>12355</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="3" t="s">
         <v>3</v>
       </c>
@@ -2014,7 +2025,7 @@
         <v>12355</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="3" t="s">
         <v>3</v>
       </c>
@@ -2035,7 +2046,7 @@
         <v>20629</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="3" t="s">
         <v>1</v>
       </c>
@@ -2056,7 +2067,7 @@
         <v>12472</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="3" t="s">
         <v>1</v>
       </c>
@@ -2077,7 +2088,7 @@
         <v>11833</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="3" t="s">
         <v>2</v>
       </c>
@@ -2098,7 +2109,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="3" t="s">
         <v>2</v>
       </c>
@@ -2119,7 +2130,7 @@
         <v>11833</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="3" t="s">
         <v>3</v>
       </c>
@@ -2140,7 +2151,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="3" t="s">
         <v>1</v>
       </c>
@@ -2161,7 +2172,7 @@
         <v>4631</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="3" t="s">
         <v>1</v>
       </c>
@@ -2182,7 +2193,7 @@
         <v>12965</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="7" t="s">
         <v>15</v>
       </c>
@@ -2203,7 +2214,7 @@
         <v>3585</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="3" t="s">
         <v>3</v>
       </c>
@@ -2224,7 +2235,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" s="3" t="s">
         <v>3</v>
       </c>
@@ -2245,7 +2256,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" s="3" t="s">
         <v>3</v>
       </c>
@@ -2266,7 +2277,7 @@
         <v>4562</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" s="3" t="s">
         <v>1</v>
       </c>
@@ -2287,7 +2298,7 @@
         <v>12472</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" s="3" t="s">
         <v>1</v>
       </c>
@@ -2308,7 +2319,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" s="3" t="s">
         <v>2</v>
       </c>
@@ -2329,7 +2340,7 @@
         <v>12965</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" s="3" t="s">
         <v>0</v>
       </c>
@@ -2350,7 +2361,7 @@
         <v>10829</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" s="3" t="s">
         <v>0</v>
       </c>
@@ -2371,7 +2382,7 @@
         <v>20629</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" s="3" t="s">
         <v>3</v>
       </c>
@@ -2392,7 +2403,7 @@
         <v>4562</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" s="3" t="s">
         <v>3</v>
       </c>
@@ -2413,7 +2424,7 @@
         <v>8972</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" s="3" t="s">
         <v>3</v>
       </c>
@@ -2434,7 +2445,7 @@
         <v>8936</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" s="3" t="s">
         <v>1</v>
       </c>
@@ -2455,7 +2466,7 @@
         <v>8936</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" s="3" t="s">
         <v>0</v>
       </c>
@@ -2476,7 +2487,7 @@
         <v>4668</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" s="3" t="s">
         <v>0</v>
       </c>
@@ -2497,7 +2508,7 @@
         <v>4631</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" s="3" t="s">
         <v>3</v>
       </c>
@@ -2518,7 +2529,7 @@
         <v>3979</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" s="3" t="s">
         <v>3</v>
       </c>
@@ -2539,7 +2550,7 @@
         <v>8701</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" s="3" t="s">
         <v>3</v>
       </c>
@@ -2560,7 +2571,7 @@
         <v>11833</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" s="3" t="s">
         <v>1</v>
       </c>
@@ -2581,7 +2592,7 @@
         <v>8701</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" s="3" t="s">
         <v>2</v>
       </c>
@@ -2602,7 +2613,7 @@
         <v>4562</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102" s="3" t="s">
         <v>2</v>
       </c>
@@ -2623,7 +2634,7 @@
         <v>8972</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103" s="3" t="s">
         <v>2</v>
       </c>
@@ -2644,7 +2655,7 @@
         <v>3979</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104" s="3" t="s">
         <v>0</v>
       </c>
@@ -2665,7 +2676,7 @@
         <v>20629</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105" s="3" t="s">
         <v>0</v>
       </c>
@@ -2686,7 +2697,7 @@
         <v>8701</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106" s="3" t="s">
         <v>0</v>
       </c>
@@ -2707,7 +2718,7 @@
         <v>12965</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107" s="3" t="s">
         <v>3</v>
       </c>
@@ -2728,7 +2739,7 @@
         <v>12355</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108" s="3" t="s">
         <v>3</v>
       </c>
@@ -2749,7 +2760,7 @@
         <v>12355</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109" s="3" t="s">
         <v>3</v>
       </c>
@@ -2770,7 +2781,7 @@
         <v>20629</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110" s="3" t="s">
         <v>1</v>
       </c>
@@ -2791,7 +2802,7 @@
         <v>12472</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A111" s="3" t="s">
         <v>1</v>
       </c>
@@ -2812,7 +2823,7 @@
         <v>11833</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A112" s="3" t="s">
         <v>2</v>
       </c>
@@ -2833,7 +2844,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A113" s="3" t="s">
         <v>2</v>
       </c>
@@ -2854,7 +2865,7 @@
         <v>11833</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A114" s="3" t="s">
         <v>3</v>
       </c>
@@ -2875,7 +2886,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A115" s="3" t="s">
         <v>1</v>
       </c>
@@ -2896,7 +2907,7 @@
         <v>4631</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A116" s="3" t="s">
         <v>1</v>
       </c>
@@ -2917,7 +2928,7 @@
         <v>12965</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A117" s="3" t="s">
         <v>0</v>
       </c>
@@ -2938,7 +2949,7 @@
         <v>6693</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A118" s="3" t="s">
         <v>0</v>
       </c>
@@ -2959,7 +2970,7 @@
         <v>8936</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A119" s="3" t="s">
         <v>0</v>
       </c>
@@ -2980,7 +2991,7 @@
         <v>12472</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A120" s="3" t="s">
         <v>3</v>
       </c>
@@ -3001,7 +3012,7 @@
         <v>3585</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A121" s="3" t="s">
         <v>3</v>
       </c>
@@ -3022,7 +3033,7 @@
         <v>3585</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A122" s="3" t="s">
         <v>3</v>
       </c>
@@ -3043,7 +3054,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A123" s="3" t="s">
         <v>3</v>
       </c>
@@ -3064,7 +3075,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A124" s="3" t="s">
         <v>3</v>
       </c>
@@ -3085,7 +3096,7 @@
         <v>4562</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A125" s="3" t="s">
         <v>1</v>
       </c>
@@ -3106,7 +3117,7 @@
         <v>12472</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A126" s="3" t="s">
         <v>1</v>
       </c>
@@ -3127,7 +3138,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A127" s="3" t="s">
         <v>2</v>
       </c>
@@ -3148,7 +3159,7 @@
         <v>12965</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A128" s="3" t="s">
         <v>0</v>
       </c>
@@ -3169,7 +3180,7 @@
         <v>10829</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A129" s="3" t="s">
         <v>0</v>
       </c>
@@ -3190,7 +3201,7 @@
         <v>20629</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A130" s="3" t="s">
         <v>3</v>
       </c>
@@ -3211,7 +3222,7 @@
         <v>4562</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A131" s="3" t="s">
         <v>3</v>
       </c>
@@ -3232,7 +3243,7 @@
         <v>8972</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A132" s="3" t="s">
         <v>3</v>
       </c>
@@ -3253,7 +3264,7 @@
         <v>8936</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A133" s="3" t="s">
         <v>1</v>
       </c>
@@ -3274,7 +3285,7 @@
         <v>8936</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A134" s="3" t="s">
         <v>0</v>
       </c>
@@ -3295,7 +3306,7 @@
         <v>4668</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A135" s="3" t="s">
         <v>0</v>
       </c>
@@ -3316,7 +3327,7 @@
         <v>4631</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A136" s="3" t="s">
         <v>3</v>
       </c>
@@ -3337,7 +3348,7 @@
         <v>3979</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A137" s="3" t="s">
         <v>3</v>
       </c>
@@ -3358,7 +3369,7 @@
         <v>8701</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A138" s="3" t="s">
         <v>3</v>
       </c>
@@ -3379,7 +3390,7 @@
         <v>11833</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A139" s="3" t="s">
         <v>1</v>
       </c>
@@ -3400,7 +3411,7 @@
         <v>8701</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A140" s="3" t="s">
         <v>2</v>
       </c>
@@ -3421,7 +3432,7 @@
         <v>4562</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A141" s="3" t="s">
         <v>2</v>
       </c>
@@ -3442,7 +3453,7 @@
         <v>8972</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A142" s="3" t="s">
         <v>2</v>
       </c>
@@ -3463,7 +3474,7 @@
         <v>3979</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A143" s="3" t="s">
         <v>0</v>
       </c>
@@ -3484,7 +3495,7 @@
         <v>20629</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A144" s="3" t="s">
         <v>0</v>
       </c>
@@ -3505,7 +3516,7 @@
         <v>8701</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A145" s="3" t="s">
         <v>0</v>
       </c>
@@ -3526,7 +3537,7 @@
         <v>12965</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A146" s="3" t="s">
         <v>3</v>
       </c>
@@ -3547,7 +3558,7 @@
         <v>12355</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A147" s="3" t="s">
         <v>3</v>
       </c>
@@ -3568,7 +3579,7 @@
         <v>12355</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A148" s="3" t="s">
         <v>3</v>
       </c>
@@ -3589,7 +3600,7 @@
         <v>20629</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A149" s="3" t="s">
         <v>1</v>
       </c>
@@ -3610,7 +3621,7 @@
         <v>12472</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A150" s="3" t="s">
         <v>1</v>
       </c>
@@ -3631,7 +3642,7 @@
         <v>11833</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A151" s="3" t="s">
         <v>2</v>
       </c>
@@ -3652,7 +3663,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A152" s="3" t="s">
         <v>2</v>
       </c>
@@ -3673,7 +3684,7 @@
         <v>11833</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A153" s="3" t="s">
         <v>3</v>
       </c>
@@ -3694,7 +3705,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A154" s="3" t="s">
         <v>1</v>
       </c>
@@ -3715,7 +3726,7 @@
         <v>4631</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A155" s="3" t="s">
         <v>1</v>
       </c>
@@ -3736,7 +3747,7 @@
         <v>12965</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A156" s="7" t="s">
         <v>15</v>
       </c>
@@ -3757,7 +3768,7 @@
         <v>3585</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A157" s="3" t="s">
         <v>3</v>
       </c>
@@ -3778,7 +3789,7 @@
         <v>1192</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A158" s="3" t="s">
         <v>3</v>
       </c>
@@ -3799,7 +3810,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A159" s="3" t="s">
         <v>3</v>
       </c>
@@ -3820,7 +3831,7 @@
         <v>4562</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A160" s="3" t="s">
         <v>1</v>
       </c>
@@ -3841,7 +3852,7 @@
         <v>12472</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A161" s="3" t="s">
         <v>1</v>
       </c>
@@ -3862,7 +3873,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A162" s="3" t="s">
         <v>2</v>
       </c>
@@ -3883,7 +3894,7 @@
         <v>12965</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A163" s="3" t="s">
         <v>0</v>
       </c>
@@ -3905,11 +3916,12 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:F42">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:F42">
     <sortCondition ref="B9"/>
   </sortState>
   <dataConsolidate/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>